<commit_message>
Mise à jour de la carte avec nouveaux sites
</commit_message>
<xml_diff>
--- a/sauvegardes/sites.xlsx
+++ b/sauvegardes/sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netestia-my.sharepoint.com/personal/adrien_mondin_etu_estia_fr/Documents/Documents/stage Terres du Sud/Analyse_surfacique/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analyse_surfacique\sauvegardes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_AD4D9D64A577C15A4A5418B180DB6DE65ADEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33DA0530-AA25-4FB4-BBD8-EBDFF9EF8B55}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2B0AA3-4186-4BE1-B6A2-D78E9499AE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="336">
   <si>
     <t>Ville</t>
   </si>
@@ -961,6 +961,78 @@
   </si>
   <si>
     <t>verteuil magasin (vendu)</t>
+  </si>
+  <si>
+    <t>souston</t>
+  </si>
+  <si>
+    <t>43.74641770860991</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1.33285379210912</t>
+  </si>
+  <si>
+    <t>mimizan</t>
+  </si>
+  <si>
+    <t>44.19725528555141</t>
+  </si>
+  <si>
+    <t>-1.2291033861765632</t>
+  </si>
+  <si>
+    <t>morcenx la nouvelle</t>
+  </si>
+  <si>
+    <t>44.02969680821508</t>
+  </si>
+  <si>
+    <t>lit et mixe</t>
+  </si>
+  <si>
+    <t>44.02549860293042</t>
+  </si>
+  <si>
+    <t>-1.2583691579531584</t>
+  </si>
+  <si>
+    <t>saint sever</t>
+  </si>
+  <si>
+    <t>43.7502878518836</t>
+  </si>
+  <si>
+    <t>-0.568674355747199</t>
+  </si>
+  <si>
+    <t>dax</t>
+  </si>
+  <si>
+    <t>43.70987517571523</t>
+  </si>
+  <si>
+    <t>-1.0441713878412118</t>
+  </si>
+  <si>
+    <t>PEYREHORADE</t>
+  </si>
+  <si>
+    <t>43.5512456094283</t>
+  </si>
+  <si>
+    <t>-1.1301652172450665</t>
+  </si>
+  <si>
+    <t>PEYREHORADE soumo</t>
+  </si>
+  <si>
+    <t>43.55076012419594</t>
+  </si>
+  <si>
+    <t>-1.1299851875293643</t>
+  </si>
+  <si>
+    <t>-0.9227099943452951</t>
   </si>
 </sst>
 </file>
@@ -1030,22 +1102,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1056,6 +1176,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6ED6C48-8A84-435B-9213-6E84A0456431}" name="Tableau1" displayName="Tableau1" ref="E7:G130" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="E7:G130" xr:uid="{E6ED6C48-8A84-435B-9213-6E84A0456431}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A7494DE9-D4C8-446E-8772-DDD82E652FCF}" name="Ville" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{15B600BA-6EF0-4976-A7F9-42F3C6BD12EF}" name="Latitude" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6CE0BFCB-2398-46F8-867A-9DF192D31C54}" name="Longitude" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1321,1264 +1453,1357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E7:G122"/>
+  <dimension ref="E7:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="36.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="1" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="1" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="1" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="1" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="1" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G80" s="1" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="88" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="89" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G89" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="90" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E90" s="2" t="s">
+      <c r="E90" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F90" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="G90" s="1" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="91" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F91" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="G91" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="92" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E92" s="2" t="s">
+      <c r="E92" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F92" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="G92" s="1" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="93" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E93" s="2" t="s">
+      <c r="E93" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F93" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="G93" s="1" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="94" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E94" s="2" t="s">
+      <c r="E94" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="F94" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="G94" s="1" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="95" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G95" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="96" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F96" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G96" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E97" s="2" t="s">
+      <c r="E97" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F97" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="G97" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="98" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E98" s="2" t="s">
+      <c r="E98" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" s="1" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E99" s="2" t="s">
+      <c r="E99" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G99" s="1" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G100" s="1" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G101" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E102" s="2" t="s">
+      <c r="E102" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" s="1" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E103" s="2" t="s">
+      <c r="E103" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F103" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G103" s="1" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E104" s="2" t="s">
+      <c r="E104" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="F104" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G104" s="1" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="105" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E105" s="2" t="s">
+      <c r="E105" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="F105" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="G105" s="1" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E106" s="2" t="s">
+      <c r="E106" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="F106" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="G106" s="1" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E107" s="2" t="s">
+      <c r="E107" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F107" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="G107" s="1" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="108" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E108" s="2" t="s">
+      <c r="E108" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F108" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G108" s="1" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E109" s="2" t="s">
+      <c r="E109" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="F109" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="G109" s="1" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E110" s="2" t="s">
+      <c r="E110" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F110" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="G110" s="1" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="111" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E111" s="2" t="s">
+      <c r="E111" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F111" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="G111" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E112" s="2" t="s">
+      <c r="E112" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F112" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="G112" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="113" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E113" s="2" t="s">
+      <c r="E113" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F113" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="G113" s="1" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="114" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
     </row>
     <row r="115" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
     </row>
     <row r="116" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F116" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G116" s="1" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="117" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E117" s="2" t="s">
+      <c r="E117" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
     </row>
     <row r="118" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E118" s="2" t="s">
+      <c r="E118" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F118" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G118" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="119" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E119" s="2" t="s">
+      <c r="E119" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F119" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="G119" s="1" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="120" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E120" s="2" t="s">
+      <c r="E120" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
     </row>
     <row r="121" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E121" s="2" t="s">
+      <c r="E121" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
     </row>
     <row r="122" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+    </row>
+    <row r="123" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E123" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="124" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E124" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="125" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E125" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="126" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E126" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="127" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E127" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="128" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E128" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="129" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E129" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E130" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>334</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>